<commit_message>
added Natanis excel, updated my own file
</commit_message>
<xml_diff>
--- a/HODANOVA/Statistics.xlsx
+++ b/HODANOVA/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\SchoolStuff\HODANOVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1A058E-E0A6-4808-81CC-72D79DDB636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC9B127-296E-4ABF-8650-76A07ADDDE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{BCCD6CBD-00C7-4E81-9EF9-9084940878AF}"/>
   </bookViews>
@@ -36,18 +36,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>BATT. VOLTAGE</t>
   </si>
   <si>
-    <t>BATT. COUNT</t>
-  </si>
-  <si>
-    <t>MODUS</t>
-  </si>
-  <si>
     <t>MEDIAN</t>
+  </si>
+  <si>
+    <t>BATT. NUM</t>
+  </si>
+  <si>
+    <t>BATT.COUNT</t>
+  </si>
+  <si>
+    <t>ARITHMETIC AVG.</t>
+  </si>
+  <si>
+    <t>LAST</t>
+  </si>
+  <si>
+    <t>FIRST</t>
+  </si>
+  <si>
+    <t>BIGGEST</t>
+  </si>
+  <si>
+    <t>SMALLEST</t>
+  </si>
+  <si>
+    <t>MODE</t>
+  </si>
+  <si>
+    <t>STANDARD DEV.</t>
+  </si>
+  <si>
+    <t>VARIENCE</t>
+  </si>
+  <si>
+    <t>RANGE</t>
   </si>
 </sst>
 </file>
@@ -63,7 +90,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,11 +109,151 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9F5EC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -95,23 +262,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCC99"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF99FFCC"/>
+      <color rgb="FFA9F5EC"/>
+      <color rgb="FFFF9999"/>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FF99FF99"/>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -440,131 +645,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56990A0E-F757-4AB9-96E2-B44F7CCE2887}">
-  <dimension ref="B2:F22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.6328125" style="1" customWidth="1"/>
-    <col min="3" max="6" width="17.6328125" customWidth="1"/>
+    <col min="1" max="2" width="17.6328125" style="1" customWidth="1"/>
+    <col min="3" max="10" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="10">
+        <v>20</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="1">
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="1">
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" s="12">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="1">
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B7" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="1">
+      <c r="C7" s="14"/>
+      <c r="E7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="1">
+      <c r="C8" s="14"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="1">
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B10" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="1">
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11" s="12">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="1">
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="1">
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" s="12">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="1">
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" s="12">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="1">
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="12">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="1">
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" s="12">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B17" s="1">
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="12">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="1">
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="12">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B19" s="1">
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="12">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B20" s="1">
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="12">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="1">
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="12">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B22" s="1">
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="2">
         <v>20</v>
       </c>
+      <c r="C22" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>